<commit_message>
send model finalize with presentation
</commit_message>
<xml_diff>
--- a/Greyform-linux-ros1/Python_Application/exporteddatassss(with TMP)(draft).xlsx
+++ b/Greyform-linux-ros1/Python_Application/exporteddatassss(with TMP)(draft).xlsx
@@ -260,7 +260,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J2" t="n">
@@ -307,7 +307,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J3" t="n">
@@ -354,7 +354,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J4" t="n">
@@ -401,7 +401,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J5" t="n">
@@ -448,7 +448,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J6" t="n">
@@ -495,7 +495,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J7" t="n">
@@ -542,7 +542,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J8" t="n">
@@ -589,7 +589,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J9" t="n">
@@ -636,7 +636,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J10" t="n">
@@ -683,7 +683,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J11" t="n">
@@ -730,7 +730,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J12" t="n">
@@ -777,7 +777,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J13" t="n">
@@ -824,7 +824,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J14" t="n">
@@ -871,7 +871,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J15" t="n">
@@ -918,7 +918,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J16" t="n">
@@ -965,7 +965,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J17" t="n">
@@ -1012,7 +1012,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J18" t="n">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J19" t="n">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J20" t="n">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J21" t="n">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J22" t="n">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J23" t="n">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J24" t="n">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>done</t>
+          <t>blank</t>
         </is>
       </c>
       <c r="J25" t="n">

</xml_diff>